<commit_message>
feat: enhance DDT stability and framework robustness
- Added data-driven tests for login and registration (valid, invalid, duplicate cases)
- Integrated ThreadLocal-safe Extent reporting
- Improved page objects with business-level actions
- Added headless execution support via configuration
- Ensured clean test state across DDT iterations
</commit_message>
<xml_diff>
--- a/testData/MOCK_DATA (1).xlsx
+++ b/testData/MOCK_DATA (1).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hp\BoomBolt_Automation\BoomBolt_Automation_Project\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3729DF2-AF66-4CEE-BF66-E61764753D78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A763BA3-C74C-4912-8FC9-878B92695203}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="95">
   <si>
     <t>username</t>
   </si>
@@ -299,6 +299,12 @@
   </si>
   <si>
     <t>kG5!MPUpJ!y)5D</t>
+  </si>
+  <si>
+    <t>expectedResultForReg</t>
+  </si>
+  <si>
+    <t>duplicate</t>
   </si>
 </sst>
 </file>
@@ -353,10 +359,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -671,10 +678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" showWhiteSpace="0" workbookViewId="0">
-      <selection sqref="A1:C31"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -682,9 +689,10 @@
     <col min="1" max="1" width="10.796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.09765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -694,8 +702,11 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -705,8 +716,11 @@
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -716,8 +730,11 @@
       <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -727,8 +744,11 @@
       <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -738,8 +758,11 @@
       <c r="C5" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
@@ -749,8 +772,11 @@
       <c r="C6" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>18</v>
       </c>
@@ -760,8 +786,11 @@
       <c r="C7" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
@@ -771,8 +800,11 @@
       <c r="C8" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>24</v>
       </c>
@@ -782,8 +814,11 @@
       <c r="C9" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>27</v>
       </c>
@@ -793,8 +828,11 @@
       <c r="C10" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>30</v>
       </c>
@@ -804,8 +842,11 @@
       <c r="C11" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>33</v>
       </c>
@@ -815,8 +856,11 @@
       <c r="C12" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>36</v>
       </c>
@@ -826,8 +870,11 @@
       <c r="C13" s="2" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>39</v>
       </c>
@@ -837,8 +884,11 @@
       <c r="C14" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>42</v>
       </c>
@@ -848,8 +898,11 @@
       <c r="C15" s="2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>45</v>
       </c>
@@ -859,8 +912,11 @@
       <c r="C16" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>48</v>
       </c>
@@ -870,8 +926,11 @@
       <c r="C17" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>51</v>
       </c>
@@ -881,8 +940,11 @@
       <c r="C18" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>54</v>
       </c>
@@ -892,8 +954,11 @@
       <c r="C19" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>57</v>
       </c>
@@ -903,8 +968,11 @@
       <c r="C20" s="2" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>60</v>
       </c>
@@ -914,8 +982,11 @@
       <c r="C21" s="2" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>63</v>
       </c>
@@ -925,8 +996,11 @@
       <c r="C22" s="2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>66</v>
       </c>
@@ -936,8 +1010,11 @@
       <c r="C23" s="2" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>69</v>
       </c>
@@ -947,8 +1024,11 @@
       <c r="C24" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>72</v>
       </c>
@@ -958,8 +1038,11 @@
       <c r="C25" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>75</v>
       </c>
@@ -969,8 +1052,11 @@
       <c r="C26" s="2" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>78</v>
       </c>
@@ -980,8 +1066,11 @@
       <c r="C27" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>81</v>
       </c>
@@ -991,8 +1080,11 @@
       <c r="C28" s="2" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>84</v>
       </c>
@@ -1002,8 +1094,11 @@
       <c r="C29" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>87</v>
       </c>
@@ -1013,8 +1108,11 @@
       <c r="C30" s="2" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>90</v>
       </c>
@@ -1024,8 +1122,12 @@
       <c r="C31" s="2" t="s">
         <v>92</v>
       </c>
+      <c r="D31" s="3" t="s">
+        <v>94</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>